<commit_message>
Improvments LI paper scripts 21st October
</commit_message>
<xml_diff>
--- a/results/tables/old/order_level_tbl.xlsx
+++ b/results/tables/old/order_level_tbl.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Order</t>
   </si>
@@ -47,25 +47,10 @@
     <t xml:space="preserve">Cichliformes</t>
   </si>
   <si>
-    <t xml:space="preserve">Clupeiformes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cypriniformes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cyprinodontiformes</t>
   </si>
   <si>
-    <t xml:space="preserve">Gymnotiformes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmoniformes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Siluriformes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synbranchiformes</t>
   </si>
 </sst>
 </file>
@@ -431,28 +416,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>1505531</v>
+        <v>1184931</v>
       </c>
       <c r="C2" t="n">
-        <v>253</v>
+        <v>145</v>
       </c>
       <c r="D2" t="n">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2" t="n">
         <v>6</v>
       </c>
-      <c r="F2" t="n">
-        <v>16</v>
-      </c>
-      <c r="G2" t="n">
-        <v>18</v>
-      </c>
-      <c r="H2" t="n">
-        <v>13</v>
-      </c>
       <c r="I2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -460,25 +445,25 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>1946427</v>
+        <v>1624714</v>
       </c>
       <c r="C3" t="n">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="D3" t="n">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -489,13 +474,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="n">
-        <v>530</v>
+        <v>3616</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -507,10 +492,10 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -518,173 +503,28 @@
         <v>12</v>
       </c>
       <c r="B5" t="n">
-        <v>4205</v>
+        <v>17755</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="n">
-        <v>6229</v>
-      </c>
-      <c r="C6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6396</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1866</v>
-      </c>
-      <c r="C8" t="n">
         <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="n">
-        <v>76560</v>
-      </c>
-      <c r="C9" t="n">
-        <v>38</v>
-      </c>
-      <c r="D9" t="n">
-        <v>29</v>
-      </c>
-      <c r="E9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F9" t="n">
-        <v>7</v>
-      </c>
-      <c r="G9" t="n">
-        <v>7</v>
-      </c>
-      <c r="H9" t="n">
-        <v>4</v>
-      </c>
-      <c r="I9" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1596</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>